<commit_message>
bm.build_sets update Optimization in model.template.py now ready to try different models rapidly
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugberk\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugberk\source\repos\Traffic Flow Speed Estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338DDF07-1F9A-4575-B7C2-6494F4F8865F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA1212B-99CC-4321-820E-BB635C4D2958}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{0A0C8B08-9AF0-49EC-B3A9-0F2C579D4185}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>